<commit_message>
addes excel file with TestCases
</commit_message>
<xml_diff>
--- a/test_back/test_forms/positive_validation_scenarious_shapes/TestCases lego_assambly_backend.xlsx
+++ b/test_back/test_forms/positive_validation_scenarious_shapes/TestCases lego_assambly_backend.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapuscasitei\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FACULTA\Anul 3\Sem 1\IA\repository assembly backend\lego-assembly-back\test_back\test_forms\positive_validation_scenarious_shapes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A981F7C-0B29-4B15-A8DA-9DC229D907ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -94,16 +95,343 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Verify "array_cubes_empty" JSON file</t>
-  </si>
-  <si>
-    <t>NEGATIVE</t>
-  </si>
-  <si>
-    <t>An error will be displayed</t>
-  </si>
-  <si>
-    <t>Apuscasitei Silviu</t>
+    <r>
+      <t xml:space="preserve">1. to have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>python application</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                            2. to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with that specifications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>github</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the application (from master)                      2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JSON file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you want to test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in the root of project </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file exist)                                                     3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cmd in the application              4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the command: python main.py THE_NAME_OF_JSON_FILE                    5. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>press</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ENTER                                          6. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from project</t>
+    </r>
+  </si>
+  <si>
+    <t>POSITIVE</t>
+  </si>
+  <si>
+    <t>No error will be displayed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEST PASSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  </t>
+    </r>
+  </si>
+  <si>
+    <t>Dima Ionut</t>
+  </si>
+  <si>
+    <t>Verify "array_cubes_nonempty" JSON file</t>
   </si>
   <si>
     <r>
@@ -128,342 +456,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> validation with an empty array of cubes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. to have the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>python application</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                            2. to have a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JSON file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with that specifications</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>download</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>github</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the application (from master)                      2. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>copy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> JSON file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> you want to test </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">in the root of project </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(where </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>main.py</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> file exist)                                                     3. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>open</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> cmd in the application              4. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>write</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the command: python main.py THE_NAME_OF_JSON_FILE                    5. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>press</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ENTER                                          6. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>delete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JSON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from project</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TEST PASSED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                  "Please provide at least 1 cube"</t>
+      <t xml:space="preserve"> validation with nonempty array of cubes</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,14 +485,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -866,40 +859,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -928,33 +921,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="G8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -965,7 +958,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -976,7 +969,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -987,7 +980,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1004,30 +997,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="63.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="54.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="54.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1063,12 +1056,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>